<commit_message>
doc: CUs terminados después de la 1era revisión
</commit_message>
<xml_diff>
--- a/Desarrollo/Artemis/Gestión y Negocio/Artemis-CP.xlsx
+++ b/Desarrollo/Artemis/Gestión y Negocio/Artemis-CP.xlsx
@@ -1,21 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ever\Desktop\UNMSM\GCS\ABSoftware\Desarrollo\Artemis\Gestión y Negocio\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FC38666-D99F-49E3-AEC8-3CAED180F633}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="19425" windowHeight="10425"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -31,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="102">
   <si>
     <t>CRONOGRAMA DEL PROYECTO</t>
   </si>
@@ -285,43 +279,64 @@
     <t>• = Alt + 7, 11pts</t>
   </si>
   <si>
-    <t>Especificación de requisito 01: Crear cuenta en Artemis</t>
-  </si>
-  <si>
-    <t>Especificación de requisito 02: Iniciar y Cerrar sesión</t>
-  </si>
-  <si>
-    <t>Especificación de requisito 03: Modificar perfil</t>
-  </si>
-  <si>
-    <t>Especificación de requisito 04: Subir una obra</t>
-  </si>
-  <si>
-    <t>Especificación de requisito 05: Comentar una obra</t>
-  </si>
-  <si>
-    <t>Especificación de requisito 06:Dar like/dislike a una obra</t>
-  </si>
-  <si>
-    <t>Especificación de requisito 07: Editar/actualizar obra</t>
-  </si>
-  <si>
-    <t>Especificación de requisito 08: Eliminar una obra propia</t>
-  </si>
-  <si>
-    <t>Especificación de requisito 09: Descargar versiones antiguas de las obras</t>
-  </si>
-  <si>
     <t>3.0</t>
   </si>
   <si>
     <t>Modificación post 1era revición</t>
+  </si>
+  <si>
+    <t>Especificación de requisito 01: Creación de Cuenta</t>
+  </si>
+  <si>
+    <t>Especificación de requisito 02: Buscar Obra o Tag</t>
+  </si>
+  <si>
+    <t>Especificación de requisito 03: Visualizar Obra</t>
+  </si>
+  <si>
+    <t>Especificación de requisito 04: Iniciar Sesión</t>
+  </si>
+  <si>
+    <t>Especificación de requisito 05: Comentar Obra</t>
+  </si>
+  <si>
+    <t>Especificación de requisito 06:Dar like o dislike a una obra</t>
+  </si>
+  <si>
+    <t>Especificación de requisito 07: Modificar Perfil</t>
+  </si>
+  <si>
+    <t>Especificación de requisito 08: Seguir a un artista</t>
+  </si>
+  <si>
+    <t>Especificación de requisito 09: Reportar Obra</t>
+  </si>
+  <si>
+    <t>Especificación de requisito 10: Cerrar Sesión</t>
+  </si>
+  <si>
+    <t>Especificación de requisito 11: Crear Obra</t>
+  </si>
+  <si>
+    <t>Especificación de requisito 12: Modificar Obra</t>
+  </si>
+  <si>
+    <t>Especificación de requisito 13: Subir nueva Versión</t>
+  </si>
+  <si>
+    <t>Especificación de requisito 14: Crear Carpeta</t>
+  </si>
+  <si>
+    <t>Especificación de requisito 15: Ver Versiones</t>
+  </si>
+  <si>
+    <t>Especificación de requisito 16: Compartir Obra</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="d/m/yyyy"/>
   </numFmts>
@@ -574,7 +589,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="65">
+  <cellXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -719,19 +734,11 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -751,6 +758,15 @@
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -966,224 +982,224 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:Q1026"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:Q1033"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="S32" sqref="S32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="6.9140625" customWidth="1"/>
-    <col min="2" max="2" width="68.9140625" customWidth="1"/>
+    <col min="1" max="1" width="6.875" customWidth="1"/>
+    <col min="2" max="2" width="68.875" customWidth="1"/>
     <col min="3" max="15" width="4" customWidth="1"/>
-    <col min="16" max="16" width="33.6640625" customWidth="1"/>
+    <col min="16" max="16" width="33.625" customWidth="1"/>
     <col min="17" max="17" width="11.25" customWidth="1"/>
-    <col min="18" max="26" width="9.4140625" customWidth="1"/>
+    <col min="18" max="26" width="9.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:17" ht="29.5">
-      <c r="B1" s="52" t="s">
+    <row r="1" spans="2:17" ht="48.75">
+      <c r="B1" s="63" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="53"/>
-      <c r="D1" s="53"/>
-      <c r="E1" s="53"/>
-      <c r="F1" s="53"/>
-      <c r="G1" s="53"/>
-      <c r="H1" s="53"/>
-      <c r="I1" s="53"/>
-      <c r="J1" s="53"/>
-      <c r="K1" s="53"/>
-      <c r="L1" s="53"/>
-      <c r="M1" s="53"/>
-      <c r="N1" s="53"/>
-      <c r="O1" s="53"/>
-      <c r="P1" s="53"/>
-      <c r="Q1" s="53"/>
-    </row>
-    <row r="2" spans="2:17" ht="14">
+      <c r="C1" s="54"/>
+      <c r="D1" s="54"/>
+      <c r="E1" s="54"/>
+      <c r="F1" s="54"/>
+      <c r="G1" s="54"/>
+      <c r="H1" s="54"/>
+      <c r="I1" s="54"/>
+      <c r="J1" s="54"/>
+      <c r="K1" s="54"/>
+      <c r="L1" s="54"/>
+      <c r="M1" s="54"/>
+      <c r="N1" s="54"/>
+      <c r="O1" s="54"/>
+      <c r="P1" s="54"/>
+      <c r="Q1" s="54"/>
+    </row>
+    <row r="2" spans="2:17" ht="18">
       <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="54" t="s">
+      <c r="C2" s="64" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="53"/>
-      <c r="E2" s="53"/>
-      <c r="F2" s="53"/>
-      <c r="G2" s="53"/>
-      <c r="H2" s="53"/>
-      <c r="I2" s="53"/>
-      <c r="J2" s="53"/>
-      <c r="K2" s="53"/>
-      <c r="L2" s="53"/>
-      <c r="M2" s="53"/>
-      <c r="N2" s="53"/>
-      <c r="O2" s="53"/>
-      <c r="P2" s="53"/>
-      <c r="Q2" s="53"/>
-    </row>
-    <row r="3" spans="2:17" ht="14">
+      <c r="D2" s="54"/>
+      <c r="E2" s="54"/>
+      <c r="F2" s="54"/>
+      <c r="G2" s="54"/>
+      <c r="H2" s="54"/>
+      <c r="I2" s="54"/>
+      <c r="J2" s="54"/>
+      <c r="K2" s="54"/>
+      <c r="L2" s="54"/>
+      <c r="M2" s="54"/>
+      <c r="N2" s="54"/>
+      <c r="O2" s="54"/>
+      <c r="P2" s="54"/>
+      <c r="Q2" s="54"/>
+    </row>
+    <row r="3" spans="2:17" ht="18">
       <c r="B3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="54" t="s">
+      <c r="C3" s="64" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="53"/>
-      <c r="E3" s="53"/>
-      <c r="F3" s="53"/>
-      <c r="G3" s="53"/>
-      <c r="H3" s="53"/>
-      <c r="I3" s="53"/>
-      <c r="J3" s="53"/>
-      <c r="K3" s="53"/>
-      <c r="L3" s="53"/>
-      <c r="M3" s="53"/>
-      <c r="N3" s="53"/>
-      <c r="O3" s="53"/>
-      <c r="P3" s="53"/>
-      <c r="Q3" s="53"/>
-    </row>
-    <row r="4" spans="2:17" ht="14">
+      <c r="D3" s="54"/>
+      <c r="E3" s="54"/>
+      <c r="F3" s="54"/>
+      <c r="G3" s="54"/>
+      <c r="H3" s="54"/>
+      <c r="I3" s="54"/>
+      <c r="J3" s="54"/>
+      <c r="K3" s="54"/>
+      <c r="L3" s="54"/>
+      <c r="M3" s="54"/>
+      <c r="N3" s="54"/>
+      <c r="O3" s="54"/>
+      <c r="P3" s="54"/>
+      <c r="Q3" s="54"/>
+    </row>
+    <row r="4" spans="2:17" ht="18">
       <c r="B4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="55" t="s">
-        <v>93</v>
-      </c>
-      <c r="D4" s="53"/>
-      <c r="E4" s="55" t="s">
-        <v>94</v>
-      </c>
-      <c r="F4" s="53"/>
-      <c r="G4" s="53"/>
-      <c r="H4" s="53"/>
-      <c r="I4" s="53"/>
-      <c r="J4" s="53"/>
-      <c r="K4" s="53"/>
-      <c r="L4" s="53"/>
-      <c r="M4" s="53"/>
-      <c r="N4" s="53"/>
-      <c r="O4" s="53"/>
-      <c r="P4" s="53"/>
-      <c r="Q4" s="53"/>
-    </row>
-    <row r="5" spans="2:17" ht="15.5">
+      <c r="C4" s="65" t="s">
+        <v>84</v>
+      </c>
+      <c r="D4" s="54"/>
+      <c r="E4" s="65" t="s">
+        <v>85</v>
+      </c>
+      <c r="F4" s="54"/>
+      <c r="G4" s="54"/>
+      <c r="H4" s="54"/>
+      <c r="I4" s="54"/>
+      <c r="J4" s="54"/>
+      <c r="K4" s="54"/>
+      <c r="L4" s="54"/>
+      <c r="M4" s="54"/>
+      <c r="N4" s="54"/>
+      <c r="O4" s="54"/>
+      <c r="P4" s="54"/>
+      <c r="Q4" s="54"/>
+    </row>
+    <row r="5" spans="2:17" ht="18.75">
       <c r="B5" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="56" t="str">
+      <c r="C5" s="53" t="str">
         <f>B12</f>
         <v>Gestión y Negocio</v>
       </c>
-      <c r="D5" s="53"/>
-      <c r="E5" s="53"/>
-      <c r="F5" s="53"/>
-      <c r="G5" s="53"/>
-      <c r="H5" s="53"/>
-      <c r="I5" s="53"/>
-      <c r="J5" s="53"/>
-      <c r="K5" s="53"/>
-      <c r="L5" s="53"/>
-      <c r="M5" s="53"/>
-      <c r="N5" s="53"/>
-      <c r="O5" s="53"/>
-      <c r="P5" s="53"/>
-      <c r="Q5" s="53"/>
-    </row>
-    <row r="6" spans="2:17" ht="15.5">
+      <c r="D5" s="54"/>
+      <c r="E5" s="54"/>
+      <c r="F5" s="54"/>
+      <c r="G5" s="54"/>
+      <c r="H5" s="54"/>
+      <c r="I5" s="54"/>
+      <c r="J5" s="54"/>
+      <c r="K5" s="54"/>
+      <c r="L5" s="54"/>
+      <c r="M5" s="54"/>
+      <c r="N5" s="54"/>
+      <c r="O5" s="54"/>
+      <c r="P5" s="54"/>
+      <c r="Q5" s="54"/>
+    </row>
+    <row r="6" spans="2:17" ht="18.75">
       <c r="B6" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="57" t="s">
+      <c r="C6" s="55" t="s">
         <v>8</v>
       </c>
-      <c r="D6" s="53"/>
-      <c r="E6" s="53"/>
-      <c r="F6" s="53"/>
-      <c r="G6" s="53"/>
-      <c r="H6" s="53"/>
-      <c r="I6" s="57" t="s">
+      <c r="D6" s="54"/>
+      <c r="E6" s="54"/>
+      <c r="F6" s="54"/>
+      <c r="G6" s="54"/>
+      <c r="H6" s="54"/>
+      <c r="I6" s="55" t="s">
         <v>9</v>
       </c>
-      <c r="J6" s="53"/>
-      <c r="K6" s="53"/>
-      <c r="L6" s="53"/>
-      <c r="M6" s="53"/>
-      <c r="N6" s="53"/>
-      <c r="O6" s="53"/>
+      <c r="J6" s="54"/>
+      <c r="K6" s="54"/>
+      <c r="L6" s="54"/>
+      <c r="M6" s="54"/>
+      <c r="N6" s="54"/>
+      <c r="O6" s="54"/>
       <c r="P6" s="4"/>
       <c r="Q6" s="4"/>
     </row>
-    <row r="7" spans="2:17" ht="15.5">
+    <row r="7" spans="2:17" ht="24.75">
       <c r="B7" s="5"/>
-      <c r="C7" s="61" t="s">
+      <c r="C7" s="59" t="s">
         <v>10</v>
       </c>
-      <c r="D7" s="53"/>
-      <c r="E7" s="53"/>
-      <c r="F7" s="53"/>
-      <c r="G7" s="53"/>
-      <c r="H7" s="53"/>
-      <c r="I7" s="61" t="s">
+      <c r="D7" s="54"/>
+      <c r="E7" s="54"/>
+      <c r="F7" s="54"/>
+      <c r="G7" s="54"/>
+      <c r="H7" s="54"/>
+      <c r="I7" s="59" t="s">
         <v>11</v>
       </c>
-      <c r="J7" s="53"/>
-      <c r="K7" s="53"/>
-      <c r="L7" s="53"/>
-      <c r="M7" s="53"/>
-      <c r="N7" s="53"/>
-      <c r="O7" s="53"/>
+      <c r="J7" s="54"/>
+      <c r="K7" s="54"/>
+      <c r="L7" s="54"/>
+      <c r="M7" s="54"/>
+      <c r="N7" s="54"/>
+      <c r="O7" s="54"/>
       <c r="P7" s="4"/>
       <c r="Q7" s="4"/>
     </row>
-    <row r="8" spans="2:17" ht="14">
+    <row r="8" spans="2:17" ht="18">
       <c r="B8" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="62">
+      <c r="C8" s="60">
         <f>DATE(2020,10,28)</f>
         <v>44132</v>
       </c>
-      <c r="D8" s="53"/>
-      <c r="E8" s="53"/>
-      <c r="F8" s="53"/>
-      <c r="G8" s="53"/>
-      <c r="H8" s="53"/>
-      <c r="I8" s="53"/>
-      <c r="J8" s="53"/>
-      <c r="K8" s="53"/>
-      <c r="L8" s="53"/>
-      <c r="M8" s="53"/>
-      <c r="N8" s="53"/>
-      <c r="O8" s="53"/>
-      <c r="P8" s="53"/>
-      <c r="Q8" s="53"/>
-    </row>
-    <row r="9" spans="2:17" ht="14">
+      <c r="D8" s="54"/>
+      <c r="E8" s="54"/>
+      <c r="F8" s="54"/>
+      <c r="G8" s="54"/>
+      <c r="H8" s="54"/>
+      <c r="I8" s="54"/>
+      <c r="J8" s="54"/>
+      <c r="K8" s="54"/>
+      <c r="L8" s="54"/>
+      <c r="M8" s="54"/>
+      <c r="N8" s="54"/>
+      <c r="O8" s="54"/>
+      <c r="P8" s="54"/>
+      <c r="Q8" s="54"/>
+    </row>
+    <row r="9" spans="2:17" ht="18">
       <c r="B9" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C9" s="63">
+      <c r="C9" s="61">
         <v>44216</v>
       </c>
-      <c r="D9" s="53"/>
-      <c r="E9" s="53"/>
-      <c r="F9" s="53"/>
-      <c r="G9" s="53"/>
-      <c r="H9" s="53"/>
-      <c r="I9" s="53"/>
-      <c r="J9" s="53"/>
-      <c r="K9" s="53"/>
-      <c r="L9" s="53"/>
-      <c r="M9" s="53"/>
-      <c r="N9" s="53"/>
-      <c r="O9" s="53"/>
-      <c r="P9" s="53"/>
-      <c r="Q9" s="53"/>
+      <c r="D9" s="54"/>
+      <c r="E9" s="54"/>
+      <c r="F9" s="54"/>
+      <c r="G9" s="54"/>
+      <c r="H9" s="54"/>
+      <c r="I9" s="54"/>
+      <c r="J9" s="54"/>
+      <c r="K9" s="54"/>
+      <c r="L9" s="54"/>
+      <c r="M9" s="54"/>
+      <c r="N9" s="54"/>
+      <c r="O9" s="54"/>
+      <c r="P9" s="54"/>
+      <c r="Q9" s="54"/>
     </row>
     <row r="10" spans="2:17" ht="19.5" customHeight="1">
       <c r="B10" s="5"/>
@@ -1253,7 +1269,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="12" spans="2:17" ht="14.5">
+    <row r="12" spans="2:17" ht="18">
       <c r="B12" s="8" t="s">
         <v>30</v>
       </c>
@@ -1273,7 +1289,7 @@
       <c r="P12" s="10"/>
       <c r="Q12" s="10"/>
     </row>
-    <row r="13" spans="2:17" ht="15.5">
+    <row r="13" spans="2:17" ht="18">
       <c r="B13" s="11" t="s">
         <v>31</v>
       </c>
@@ -1301,7 +1317,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="2:17" ht="14.5">
+    <row r="14" spans="2:17" ht="18">
       <c r="B14" s="16" t="s">
         <v>34</v>
       </c>
@@ -1325,7 +1341,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="2:17" ht="14.5">
+    <row r="15" spans="2:17" ht="18">
       <c r="B15" s="16" t="s">
         <v>36</v>
       </c>
@@ -1349,7 +1365,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="2:17" ht="14.5">
+    <row r="16" spans="2:17" ht="18">
       <c r="B16" s="19" t="s">
         <v>37</v>
       </c>
@@ -1373,7 +1389,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="2:17" ht="14.5">
+    <row r="17" spans="2:17" ht="18">
       <c r="B17" s="19" t="s">
         <v>38</v>
       </c>
@@ -1397,7 +1413,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="2:17" ht="14.5">
+    <row r="18" spans="2:17" ht="18">
       <c r="B18" s="19" t="s">
         <v>39</v>
       </c>
@@ -1421,7 +1437,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="2:17" ht="15.5">
+    <row r="19" spans="2:17" ht="18">
       <c r="B19" s="11" t="s">
         <v>40</v>
       </c>
@@ -1447,7 +1463,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="2:17" ht="15.5">
+    <row r="20" spans="2:17" ht="18">
       <c r="B20" s="11" t="s">
         <v>42</v>
       </c>
@@ -1475,27 +1491,27 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="2:17" ht="14">
-      <c r="B21" s="64" t="s">
+    <row r="21" spans="2:17" ht="24">
+      <c r="B21" s="62" t="s">
         <v>44</v>
       </c>
-      <c r="C21" s="59"/>
-      <c r="D21" s="59"/>
-      <c r="E21" s="59"/>
-      <c r="F21" s="59"/>
-      <c r="G21" s="59"/>
-      <c r="H21" s="59"/>
-      <c r="I21" s="59"/>
-      <c r="J21" s="59"/>
-      <c r="K21" s="59"/>
-      <c r="L21" s="59"/>
-      <c r="M21" s="59"/>
-      <c r="N21" s="59"/>
-      <c r="O21" s="59"/>
-      <c r="P21" s="59"/>
-      <c r="Q21" s="60"/>
-    </row>
-    <row r="22" spans="2:17" ht="14">
+      <c r="C21" s="57"/>
+      <c r="D21" s="57"/>
+      <c r="E21" s="57"/>
+      <c r="F21" s="57"/>
+      <c r="G21" s="57"/>
+      <c r="H21" s="57"/>
+      <c r="I21" s="57"/>
+      <c r="J21" s="57"/>
+      <c r="K21" s="57"/>
+      <c r="L21" s="57"/>
+      <c r="M21" s="57"/>
+      <c r="N21" s="57"/>
+      <c r="O21" s="57"/>
+      <c r="P21" s="57"/>
+      <c r="Q21" s="58"/>
+    </row>
+    <row r="22" spans="2:17" ht="18">
       <c r="B22" s="8" t="s">
         <v>45</v>
       </c>
@@ -1515,13 +1531,15 @@
       <c r="P22" s="23"/>
       <c r="Q22" s="23"/>
     </row>
-    <row r="23" spans="2:17" ht="15.5">
+    <row r="23" spans="2:17" ht="18">
       <c r="B23" s="30" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="C23" s="12"/>
       <c r="D23" s="12"/>
-      <c r="E23" s="25"/>
+      <c r="E23" s="33" t="s">
+        <v>32</v>
+      </c>
       <c r="F23" s="25"/>
       <c r="G23" s="24"/>
       <c r="H23" s="20"/>
@@ -1539,13 +1557,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="2:17" ht="15.5">
+    <row r="24" spans="2:17" ht="18">
       <c r="B24" s="31" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="C24" s="12"/>
       <c r="D24" s="12"/>
-      <c r="E24" s="25"/>
+      <c r="E24" s="33" t="s">
+        <v>32</v>
+      </c>
       <c r="F24" s="25"/>
       <c r="G24" s="24"/>
       <c r="H24" s="20"/>
@@ -1563,13 +1583,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="2:17" ht="15.5">
+    <row r="25" spans="2:17" ht="18">
       <c r="B25" s="30" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="C25" s="12"/>
       <c r="D25" s="12"/>
-      <c r="E25" s="25"/>
+      <c r="E25" s="33" t="s">
+        <v>32</v>
+      </c>
       <c r="F25" s="25"/>
       <c r="G25" s="24"/>
       <c r="H25" s="20"/>
@@ -1587,13 +1609,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="2:17" ht="15.5">
+    <row r="26" spans="2:17" ht="18">
       <c r="B26" s="30" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="C26" s="12"/>
       <c r="D26" s="12"/>
-      <c r="E26" s="25"/>
+      <c r="E26" s="33" t="s">
+        <v>32</v>
+      </c>
       <c r="F26" s="25"/>
       <c r="G26" s="24"/>
       <c r="H26" s="20"/>
@@ -1611,13 +1635,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="2:17" ht="15.5">
+    <row r="27" spans="2:17" ht="18">
       <c r="B27" s="30" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="C27" s="12"/>
       <c r="D27" s="12"/>
-      <c r="E27" s="25"/>
+      <c r="E27" s="33" t="s">
+        <v>32</v>
+      </c>
       <c r="F27" s="25"/>
       <c r="G27" s="24"/>
       <c r="H27" s="20"/>
@@ -1635,13 +1661,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="2:17" ht="15.5">
+    <row r="28" spans="2:17" ht="18">
       <c r="B28" s="30" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="C28" s="12"/>
       <c r="D28" s="12"/>
-      <c r="E28" s="25"/>
+      <c r="E28" s="33" t="s">
+        <v>32</v>
+      </c>
       <c r="F28" s="25"/>
       <c r="G28" s="24"/>
       <c r="H28" s="20"/>
@@ -1659,13 +1687,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="2:17" ht="15.5">
+    <row r="29" spans="2:17" ht="18">
       <c r="B29" s="30" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="C29" s="12"/>
       <c r="D29" s="12"/>
-      <c r="E29" s="25"/>
+      <c r="E29" s="33" t="s">
+        <v>32</v>
+      </c>
       <c r="F29" s="25"/>
       <c r="G29" s="24"/>
       <c r="H29" s="20"/>
@@ -1683,13 +1713,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="2:17" ht="15.5">
+    <row r="30" spans="2:17" ht="18">
       <c r="B30" s="30" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="C30" s="12"/>
       <c r="D30" s="12"/>
-      <c r="E30" s="25"/>
+      <c r="E30" s="33" t="s">
+        <v>32</v>
+      </c>
       <c r="F30" s="25"/>
       <c r="G30" s="24"/>
       <c r="H30" s="20"/>
@@ -1707,14 +1739,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="2:17" ht="15.5">
+    <row r="31" spans="2:17" ht="18">
       <c r="B31" s="30" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="C31" s="12"/>
       <c r="D31" s="12"/>
       <c r="E31" s="25"/>
-      <c r="F31" s="25"/>
+      <c r="F31" s="33" t="s">
+        <v>32</v>
+      </c>
       <c r="G31" s="24"/>
       <c r="H31" s="20"/>
       <c r="I31" s="12"/>
@@ -1731,359 +1765,401 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="2:17" ht="15.5">
-      <c r="B32" s="30" t="s">
-        <v>46</v>
-      </c>
-      <c r="C32" s="12"/>
-      <c r="D32" s="12"/>
-      <c r="E32" s="33" t="s">
+    <row r="32" spans="2:17" s="52" customFormat="1" ht="18">
+      <c r="B32" s="42" t="s">
+        <v>95</v>
+      </c>
+      <c r="C32" s="20"/>
+      <c r="D32" s="20"/>
+      <c r="E32" s="25"/>
+      <c r="F32" s="33" t="s">
         <v>32</v>
       </c>
-      <c r="F32" s="24"/>
       <c r="G32" s="24"/>
       <c r="H32" s="20"/>
-      <c r="I32" s="12"/>
-      <c r="J32" s="12"/>
-      <c r="K32" s="12"/>
-      <c r="L32" s="12"/>
-      <c r="M32" s="12"/>
-      <c r="N32" s="12"/>
-      <c r="O32" s="12"/>
-      <c r="P32" s="14" t="s">
-        <v>47</v>
+      <c r="I32" s="20"/>
+      <c r="J32" s="20"/>
+      <c r="K32" s="20"/>
+      <c r="L32" s="20"/>
+      <c r="M32" s="20"/>
+      <c r="N32" s="20"/>
+      <c r="O32" s="20"/>
+      <c r="P32" s="42" t="s">
+        <v>43</v>
       </c>
       <c r="Q32" s="18">
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="2:17" ht="15.5">
-      <c r="B33" s="27" t="s">
-        <v>48</v>
-      </c>
-      <c r="C33" s="12"/>
-      <c r="D33" s="12"/>
-      <c r="E33" s="29" t="s">
-        <v>35</v>
-      </c>
-      <c r="F33" s="24"/>
+    <row r="33" spans="2:17" s="52" customFormat="1" ht="18">
+      <c r="B33" s="42" t="s">
+        <v>96</v>
+      </c>
+      <c r="C33" s="20"/>
+      <c r="D33" s="20"/>
+      <c r="E33" s="25"/>
+      <c r="F33" s="33" t="s">
+        <v>32</v>
+      </c>
       <c r="G33" s="24"/>
       <c r="H33" s="20"/>
-      <c r="I33" s="12"/>
-      <c r="J33" s="12"/>
-      <c r="K33" s="12"/>
-      <c r="L33" s="12"/>
-      <c r="M33" s="12"/>
-      <c r="N33" s="12"/>
-      <c r="O33" s="12"/>
-      <c r="P33" s="14"/>
+      <c r="I33" s="20"/>
+      <c r="J33" s="20"/>
+      <c r="K33" s="20"/>
+      <c r="L33" s="20"/>
+      <c r="M33" s="20"/>
+      <c r="N33" s="20"/>
+      <c r="O33" s="20"/>
+      <c r="P33" s="42" t="s">
+        <v>43</v>
+      </c>
       <c r="Q33" s="18">
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="2:17" ht="15.5">
-      <c r="B34" s="27" t="s">
-        <v>49</v>
-      </c>
-      <c r="C34" s="12"/>
-      <c r="D34" s="12"/>
-      <c r="E34" s="29" t="s">
-        <v>35</v>
-      </c>
-      <c r="F34" s="24"/>
+    <row r="34" spans="2:17" s="52" customFormat="1" ht="18">
+      <c r="B34" s="42" t="s">
+        <v>97</v>
+      </c>
+      <c r="C34" s="20"/>
+      <c r="D34" s="20"/>
+      <c r="E34" s="25"/>
+      <c r="F34" s="33" t="s">
+        <v>32</v>
+      </c>
       <c r="G34" s="24"/>
       <c r="H34" s="20"/>
-      <c r="I34" s="12"/>
-      <c r="J34" s="12"/>
-      <c r="K34" s="12"/>
-      <c r="L34" s="12"/>
-      <c r="M34" s="12"/>
-      <c r="N34" s="12"/>
-      <c r="O34" s="12"/>
-      <c r="P34" s="14"/>
+      <c r="I34" s="20"/>
+      <c r="J34" s="20"/>
+      <c r="K34" s="20"/>
+      <c r="L34" s="20"/>
+      <c r="M34" s="20"/>
+      <c r="N34" s="20"/>
+      <c r="O34" s="20"/>
+      <c r="P34" s="42" t="s">
+        <v>43</v>
+      </c>
       <c r="Q34" s="18">
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="2:17" ht="15.5">
-      <c r="B35" s="14" t="s">
-        <v>50</v>
-      </c>
-      <c r="C35" s="12"/>
-      <c r="D35" s="12"/>
-      <c r="E35" s="20"/>
-      <c r="F35" s="25"/>
-      <c r="G35" s="25"/>
-      <c r="H35" s="26"/>
-      <c r="I35" s="12"/>
-      <c r="J35" s="12"/>
-      <c r="K35" s="12"/>
-      <c r="L35" s="12"/>
-      <c r="M35" s="12"/>
-      <c r="N35" s="12"/>
-      <c r="O35" s="12"/>
-      <c r="P35" s="14" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q35" s="15">
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="36" spans="2:17" ht="15.5">
-      <c r="B36" s="14" t="s">
-        <v>52</v>
-      </c>
-      <c r="C36" s="12"/>
-      <c r="D36" s="12"/>
-      <c r="E36" s="12"/>
-      <c r="F36" s="25"/>
-      <c r="G36" s="25"/>
-      <c r="H36" s="34"/>
-      <c r="I36" s="12"/>
-      <c r="J36" s="12"/>
-      <c r="K36" s="12"/>
-      <c r="L36" s="12"/>
-      <c r="M36" s="12"/>
-      <c r="N36" s="12"/>
-      <c r="O36" s="12"/>
-      <c r="P36" s="14" t="s">
-        <v>53</v>
-      </c>
-      <c r="Q36" s="15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="2:17" ht="15.5">
-      <c r="B37" s="27" t="s">
-        <v>54</v>
-      </c>
-      <c r="C37" s="12"/>
-      <c r="D37" s="12"/>
-      <c r="E37" s="12"/>
-      <c r="F37" s="29"/>
-      <c r="G37" s="29"/>
-      <c r="H37" s="28"/>
-      <c r="I37" s="35"/>
-      <c r="J37" s="12"/>
-      <c r="K37" s="12"/>
-      <c r="L37" s="12"/>
-      <c r="M37" s="12"/>
-      <c r="N37" s="12"/>
-      <c r="O37" s="12"/>
-      <c r="P37" s="14" t="s">
+    <row r="35" spans="2:17" s="52" customFormat="1" ht="18">
+      <c r="B35" s="42" t="s">
+        <v>98</v>
+      </c>
+      <c r="C35" s="20"/>
+      <c r="D35" s="20"/>
+      <c r="E35" s="25"/>
+      <c r="F35" s="33" t="s">
+        <v>32</v>
+      </c>
+      <c r="G35" s="24"/>
+      <c r="H35" s="20"/>
+      <c r="I35" s="20"/>
+      <c r="J35" s="20"/>
+      <c r="K35" s="20"/>
+      <c r="L35" s="20"/>
+      <c r="M35" s="20"/>
+      <c r="N35" s="20"/>
+      <c r="O35" s="20"/>
+      <c r="P35" s="42" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q35" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="2:17" s="52" customFormat="1" ht="18">
+      <c r="B36" s="42" t="s">
+        <v>99</v>
+      </c>
+      <c r="C36" s="20"/>
+      <c r="D36" s="20"/>
+      <c r="E36" s="25"/>
+      <c r="F36" s="33" t="s">
+        <v>32</v>
+      </c>
+      <c r="G36" s="24"/>
+      <c r="H36" s="20"/>
+      <c r="I36" s="20"/>
+      <c r="J36" s="20"/>
+      <c r="K36" s="20"/>
+      <c r="L36" s="20"/>
+      <c r="M36" s="20"/>
+      <c r="N36" s="20"/>
+      <c r="O36" s="20"/>
+      <c r="P36" s="42" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q36" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="2:17" s="52" customFormat="1" ht="18">
+      <c r="B37" s="42" t="s">
+        <v>100</v>
+      </c>
+      <c r="C37" s="20"/>
+      <c r="D37" s="20"/>
+      <c r="E37" s="25"/>
+      <c r="F37" s="33" t="s">
+        <v>32</v>
+      </c>
+      <c r="G37" s="24"/>
+      <c r="H37" s="20"/>
+      <c r="I37" s="20"/>
+      <c r="J37" s="20"/>
+      <c r="K37" s="20"/>
+      <c r="L37" s="20"/>
+      <c r="M37" s="20"/>
+      <c r="N37" s="20"/>
+      <c r="O37" s="20"/>
+      <c r="P37" s="42" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q37" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="2:17" s="52" customFormat="1" ht="18">
+      <c r="B38" s="42" t="s">
+        <v>101</v>
+      </c>
+      <c r="C38" s="20"/>
+      <c r="D38" s="20"/>
+      <c r="E38" s="25"/>
+      <c r="F38" s="33" t="s">
+        <v>32</v>
+      </c>
+      <c r="G38" s="24"/>
+      <c r="H38" s="20"/>
+      <c r="I38" s="20"/>
+      <c r="J38" s="20"/>
+      <c r="K38" s="20"/>
+      <c r="L38" s="20"/>
+      <c r="M38" s="20"/>
+      <c r="N38" s="20"/>
+      <c r="O38" s="20"/>
+      <c r="P38" s="42" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q38" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="2:17" ht="18">
+      <c r="B39" s="30" t="s">
+        <v>46</v>
+      </c>
+      <c r="C39" s="12"/>
+      <c r="D39" s="12"/>
+      <c r="E39" s="33" t="s">
+        <v>32</v>
+      </c>
+      <c r="F39" s="24"/>
+      <c r="G39" s="24"/>
+      <c r="H39" s="20"/>
+      <c r="I39" s="12"/>
+      <c r="J39" s="12"/>
+      <c r="K39" s="12"/>
+      <c r="L39" s="12"/>
+      <c r="M39" s="12"/>
+      <c r="N39" s="12"/>
+      <c r="O39" s="12"/>
+      <c r="P39" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="Q37" s="15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="2:17" ht="15.5">
-      <c r="B38" s="14" t="s">
-        <v>55</v>
-      </c>
-      <c r="C38" s="12"/>
-      <c r="D38" s="12"/>
-      <c r="E38" s="12"/>
-      <c r="F38" s="36"/>
-      <c r="G38" s="36"/>
-      <c r="H38" s="26"/>
-      <c r="I38" s="34"/>
-      <c r="J38" s="12"/>
-      <c r="K38" s="12"/>
-      <c r="L38" s="12"/>
-      <c r="M38" s="12"/>
-      <c r="N38" s="12"/>
-      <c r="O38" s="12"/>
-      <c r="P38" s="14" t="s">
-        <v>56</v>
-      </c>
-      <c r="Q38" s="15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="2:17" ht="14">
-      <c r="B39" s="58" t="s">
-        <v>57</v>
-      </c>
-      <c r="C39" s="59"/>
-      <c r="D39" s="59"/>
-      <c r="E39" s="59"/>
-      <c r="F39" s="59"/>
-      <c r="G39" s="59"/>
-      <c r="H39" s="59"/>
-      <c r="I39" s="59"/>
-      <c r="J39" s="59"/>
-      <c r="K39" s="59"/>
-      <c r="L39" s="59"/>
-      <c r="M39" s="59"/>
-      <c r="N39" s="59"/>
-      <c r="O39" s="59"/>
-      <c r="P39" s="59"/>
-      <c r="Q39" s="60"/>
-    </row>
-    <row r="40" spans="2:17" ht="14">
-      <c r="B40" s="37" t="s">
-        <v>58</v>
-      </c>
-      <c r="C40" s="38"/>
-      <c r="D40" s="38"/>
-      <c r="E40" s="38"/>
-      <c r="F40" s="38"/>
-      <c r="G40" s="38"/>
-      <c r="H40" s="38"/>
-      <c r="I40" s="38"/>
-      <c r="J40" s="38"/>
-      <c r="K40" s="38"/>
-      <c r="L40" s="38"/>
-      <c r="M40" s="38"/>
-      <c r="N40" s="38"/>
-      <c r="O40" s="38"/>
-      <c r="P40" s="39"/>
-      <c r="Q40" s="39"/>
-    </row>
-    <row r="41" spans="2:17" ht="15.5">
-      <c r="B41" s="14" t="s">
-        <v>59</v>
+      <c r="Q39" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="2:17" ht="18">
+      <c r="B40" s="27" t="s">
+        <v>48</v>
+      </c>
+      <c r="C40" s="12"/>
+      <c r="D40" s="12"/>
+      <c r="E40" s="29" t="s">
+        <v>35</v>
+      </c>
+      <c r="F40" s="24"/>
+      <c r="G40" s="24"/>
+      <c r="H40" s="20"/>
+      <c r="I40" s="12"/>
+      <c r="J40" s="12"/>
+      <c r="K40" s="12"/>
+      <c r="L40" s="12"/>
+      <c r="M40" s="12"/>
+      <c r="N40" s="12"/>
+      <c r="O40" s="12"/>
+      <c r="P40" s="14"/>
+      <c r="Q40" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="2:17" ht="18">
+      <c r="B41" s="27" t="s">
+        <v>49</v>
       </c>
       <c r="C41" s="12"/>
       <c r="D41" s="12"/>
-      <c r="E41" s="12"/>
-      <c r="F41" s="12"/>
-      <c r="G41" s="36"/>
-      <c r="H41" s="36"/>
-      <c r="I41" s="36"/>
-      <c r="J41" s="36"/>
-      <c r="K41" s="40"/>
-      <c r="L41" s="40"/>
-      <c r="M41" s="41"/>
-      <c r="N41" s="41"/>
+      <c r="E41" s="29" t="s">
+        <v>35</v>
+      </c>
+      <c r="F41" s="24"/>
+      <c r="G41" s="24"/>
+      <c r="H41" s="20"/>
+      <c r="I41" s="12"/>
+      <c r="J41" s="12"/>
+      <c r="K41" s="12"/>
+      <c r="L41" s="12"/>
+      <c r="M41" s="12"/>
+      <c r="N41" s="12"/>
       <c r="O41" s="12"/>
       <c r="P41" s="14"/>
-      <c r="Q41" s="42"/>
-    </row>
-    <row r="42" spans="2:17" ht="15.5">
+      <c r="Q41" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="2:17" ht="18">
       <c r="B42" s="14" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="C42" s="12"/>
       <c r="D42" s="12"/>
-      <c r="E42" s="12"/>
-      <c r="F42" s="12"/>
-      <c r="G42" s="36"/>
-      <c r="H42" s="36"/>
-      <c r="I42" s="36"/>
-      <c r="J42" s="36"/>
-      <c r="K42" s="40"/>
-      <c r="L42" s="40"/>
-      <c r="M42" s="41"/>
-      <c r="N42" s="41"/>
+      <c r="E42" s="20"/>
+      <c r="F42" s="25"/>
+      <c r="G42" s="25"/>
+      <c r="H42" s="26"/>
+      <c r="I42" s="12"/>
+      <c r="J42" s="12"/>
+      <c r="K42" s="12"/>
+      <c r="L42" s="12"/>
+      <c r="M42" s="12"/>
+      <c r="N42" s="12"/>
       <c r="O42" s="12"/>
-      <c r="P42" s="14"/>
-      <c r="Q42" s="42"/>
-    </row>
-    <row r="43" spans="2:17" ht="15.5">
+      <c r="P42" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q42" s="15">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="43" spans="2:17" ht="18">
       <c r="B43" s="14" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="C43" s="12"/>
       <c r="D43" s="12"/>
       <c r="E43" s="12"/>
-      <c r="F43" s="12"/>
-      <c r="G43" s="36"/>
-      <c r="H43" s="36"/>
-      <c r="I43" s="36"/>
-      <c r="J43" s="36"/>
-      <c r="K43" s="40"/>
-      <c r="L43" s="40"/>
-      <c r="M43" s="41"/>
-      <c r="N43" s="41"/>
+      <c r="F43" s="25"/>
+      <c r="G43" s="25"/>
+      <c r="H43" s="34"/>
+      <c r="I43" s="12"/>
+      <c r="J43" s="12"/>
+      <c r="K43" s="12"/>
+      <c r="L43" s="12"/>
+      <c r="M43" s="12"/>
+      <c r="N43" s="12"/>
       <c r="O43" s="12"/>
-      <c r="P43" s="14"/>
-      <c r="Q43" s="42"/>
-    </row>
-    <row r="44" spans="2:17" ht="15.5">
-      <c r="B44" s="14" t="s">
-        <v>62</v>
+      <c r="P43" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="Q43" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="2:17" ht="18">
+      <c r="B44" s="27" t="s">
+        <v>54</v>
       </c>
       <c r="C44" s="12"/>
       <c r="D44" s="12"/>
       <c r="E44" s="12"/>
-      <c r="F44" s="12"/>
-      <c r="G44" s="36"/>
-      <c r="H44" s="36"/>
-      <c r="I44" s="36"/>
-      <c r="J44" s="36"/>
-      <c r="K44" s="40"/>
-      <c r="L44" s="40"/>
-      <c r="M44" s="41"/>
-      <c r="N44" s="41"/>
+      <c r="F44" s="29"/>
+      <c r="G44" s="29"/>
+      <c r="H44" s="28"/>
+      <c r="I44" s="35"/>
+      <c r="J44" s="12"/>
+      <c r="K44" s="12"/>
+      <c r="L44" s="12"/>
+      <c r="M44" s="12"/>
+      <c r="N44" s="12"/>
       <c r="O44" s="12"/>
-      <c r="P44" s="14"/>
-      <c r="Q44" s="42"/>
-    </row>
-    <row r="45" spans="2:17" ht="15.5">
+      <c r="P44" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="Q44" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="2:17" ht="18">
       <c r="B45" s="14" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="C45" s="12"/>
       <c r="D45" s="12"/>
       <c r="E45" s="12"/>
-      <c r="F45" s="12"/>
+      <c r="F45" s="36"/>
       <c r="G45" s="36"/>
-      <c r="H45" s="36"/>
-      <c r="I45" s="36"/>
-      <c r="J45" s="36"/>
-      <c r="K45" s="40"/>
-      <c r="L45" s="40"/>
-      <c r="M45" s="41"/>
-      <c r="N45" s="41"/>
+      <c r="H45" s="26"/>
+      <c r="I45" s="34"/>
+      <c r="J45" s="12"/>
+      <c r="K45" s="12"/>
+      <c r="L45" s="12"/>
+      <c r="M45" s="12"/>
+      <c r="N45" s="12"/>
       <c r="O45" s="12"/>
-      <c r="P45" s="14"/>
-      <c r="Q45" s="42"/>
-    </row>
-    <row r="46" spans="2:17" ht="15.5">
-      <c r="B46" s="14" t="s">
-        <v>64</v>
-      </c>
-      <c r="C46" s="12"/>
-      <c r="D46" s="12"/>
-      <c r="E46" s="12"/>
-      <c r="F46" s="12"/>
-      <c r="G46" s="36"/>
-      <c r="H46" s="36"/>
-      <c r="I46" s="36"/>
-      <c r="J46" s="36"/>
-      <c r="K46" s="40"/>
-      <c r="L46" s="40"/>
-      <c r="M46" s="41"/>
-      <c r="N46" s="41"/>
-      <c r="O46" s="12"/>
-      <c r="P46" s="14"/>
-      <c r="Q46" s="42"/>
-    </row>
-    <row r="47" spans="2:17" ht="15.5">
-      <c r="B47" s="14" t="s">
-        <v>65</v>
-      </c>
-      <c r="C47" s="12"/>
-      <c r="D47" s="12"/>
-      <c r="E47" s="12"/>
-      <c r="F47" s="12"/>
-      <c r="G47" s="36"/>
-      <c r="H47" s="36"/>
-      <c r="I47" s="36"/>
-      <c r="J47" s="36"/>
-      <c r="K47" s="40"/>
-      <c r="L47" s="40"/>
-      <c r="M47" s="41"/>
-      <c r="N47" s="41"/>
-      <c r="O47" s="12"/>
-      <c r="P47" s="14"/>
-      <c r="Q47" s="42"/>
-    </row>
-    <row r="48" spans="2:17" ht="15.5">
+      <c r="P45" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="Q45" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="2:17" ht="20.25">
+      <c r="B46" s="56" t="s">
+        <v>57</v>
+      </c>
+      <c r="C46" s="57"/>
+      <c r="D46" s="57"/>
+      <c r="E46" s="57"/>
+      <c r="F46" s="57"/>
+      <c r="G46" s="57"/>
+      <c r="H46" s="57"/>
+      <c r="I46" s="57"/>
+      <c r="J46" s="57"/>
+      <c r="K46" s="57"/>
+      <c r="L46" s="57"/>
+      <c r="M46" s="57"/>
+      <c r="N46" s="57"/>
+      <c r="O46" s="57"/>
+      <c r="P46" s="57"/>
+      <c r="Q46" s="58"/>
+    </row>
+    <row r="47" spans="2:17" ht="18">
+      <c r="B47" s="37" t="s">
+        <v>58</v>
+      </c>
+      <c r="C47" s="38"/>
+      <c r="D47" s="38"/>
+      <c r="E47" s="38"/>
+      <c r="F47" s="38"/>
+      <c r="G47" s="38"/>
+      <c r="H47" s="38"/>
+      <c r="I47" s="38"/>
+      <c r="J47" s="38"/>
+      <c r="K47" s="38"/>
+      <c r="L47" s="38"/>
+      <c r="M47" s="38"/>
+      <c r="N47" s="38"/>
+      <c r="O47" s="38"/>
+      <c r="P47" s="39"/>
+      <c r="Q47" s="39"/>
+    </row>
+    <row r="48" spans="2:17" ht="18">
       <c r="B48" s="14" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="C48" s="12"/>
       <c r="D48" s="12"/>
@@ -2101,9 +2177,9 @@
       <c r="P48" s="14"/>
       <c r="Q48" s="42"/>
     </row>
-    <row r="49" spans="2:17" ht="15.75" customHeight="1">
+    <row r="49" spans="2:17" ht="18">
       <c r="B49" s="14" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="C49" s="12"/>
       <c r="D49" s="12"/>
@@ -2118,34 +2194,32 @@
       <c r="M49" s="41"/>
       <c r="N49" s="41"/>
       <c r="O49" s="12"/>
-      <c r="P49" s="43" t="s">
-        <v>68</v>
-      </c>
+      <c r="P49" s="14"/>
       <c r="Q49" s="42"/>
     </row>
-    <row r="50" spans="2:17" ht="15.75" customHeight="1">
-      <c r="B50" s="37" t="s">
-        <v>69</v>
-      </c>
-      <c r="C50" s="44"/>
-      <c r="D50" s="44"/>
-      <c r="E50" s="44"/>
-      <c r="F50" s="44"/>
-      <c r="G50" s="44"/>
-      <c r="H50" s="44"/>
-      <c r="I50" s="44"/>
-      <c r="J50" s="44"/>
-      <c r="K50" s="44"/>
-      <c r="L50" s="44"/>
-      <c r="M50" s="44"/>
-      <c r="N50" s="44"/>
-      <c r="O50" s="44"/>
-      <c r="P50" s="45"/>
-      <c r="Q50" s="45"/>
-    </row>
-    <row r="51" spans="2:17" ht="15.75" customHeight="1">
+    <row r="50" spans="2:17" ht="18">
+      <c r="B50" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="C50" s="12"/>
+      <c r="D50" s="12"/>
+      <c r="E50" s="12"/>
+      <c r="F50" s="12"/>
+      <c r="G50" s="36"/>
+      <c r="H50" s="36"/>
+      <c r="I50" s="36"/>
+      <c r="J50" s="36"/>
+      <c r="K50" s="40"/>
+      <c r="L50" s="40"/>
+      <c r="M50" s="41"/>
+      <c r="N50" s="41"/>
+      <c r="O50" s="12"/>
+      <c r="P50" s="14"/>
+      <c r="Q50" s="42"/>
+    </row>
+    <row r="51" spans="2:17" ht="18">
       <c r="B51" s="14" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="C51" s="12"/>
       <c r="D51" s="12"/>
@@ -2160,14 +2234,12 @@
       <c r="M51" s="41"/>
       <c r="N51" s="41"/>
       <c r="O51" s="12"/>
-      <c r="P51" s="14" t="s">
-        <v>71</v>
-      </c>
+      <c r="P51" s="14"/>
       <c r="Q51" s="42"/>
     </row>
-    <row r="52" spans="2:17" ht="15.75" customHeight="1">
-      <c r="B52" s="27" t="s">
-        <v>72</v>
+    <row r="52" spans="2:17" ht="18">
+      <c r="B52" s="14" t="s">
+        <v>63</v>
       </c>
       <c r="C52" s="12"/>
       <c r="D52" s="12"/>
@@ -2185,9 +2257,9 @@
       <c r="P52" s="14"/>
       <c r="Q52" s="42"/>
     </row>
-    <row r="53" spans="2:17" ht="15.75" customHeight="1">
-      <c r="B53" s="27" t="s">
-        <v>73</v>
+    <row r="53" spans="2:17" ht="18">
+      <c r="B53" s="14" t="s">
+        <v>64</v>
       </c>
       <c r="C53" s="12"/>
       <c r="D53" s="12"/>
@@ -2205,9 +2277,9 @@
       <c r="P53" s="14"/>
       <c r="Q53" s="42"/>
     </row>
-    <row r="54" spans="2:17" ht="15.75" customHeight="1">
-      <c r="B54" s="27" t="s">
-        <v>74</v>
+    <row r="54" spans="2:17" ht="18">
+      <c r="B54" s="14" t="s">
+        <v>65</v>
       </c>
       <c r="C54" s="12"/>
       <c r="D54" s="12"/>
@@ -2225,175 +2297,312 @@
       <c r="P54" s="14"/>
       <c r="Q54" s="42"/>
     </row>
-    <row r="55" spans="2:17" ht="15.75" customHeight="1">
-      <c r="B55" s="58" t="s">
-        <v>75</v>
-      </c>
-      <c r="C55" s="59"/>
-      <c r="D55" s="59"/>
-      <c r="E55" s="59"/>
-      <c r="F55" s="59"/>
-      <c r="G55" s="59"/>
-      <c r="H55" s="59"/>
-      <c r="I55" s="59"/>
-      <c r="J55" s="59"/>
-      <c r="K55" s="59"/>
-      <c r="L55" s="59"/>
-      <c r="M55" s="59"/>
-      <c r="N55" s="59"/>
-      <c r="O55" s="59"/>
-      <c r="P55" s="59"/>
-      <c r="Q55" s="60"/>
+    <row r="55" spans="2:17" ht="18">
+      <c r="B55" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="C55" s="12"/>
+      <c r="D55" s="12"/>
+      <c r="E55" s="12"/>
+      <c r="F55" s="12"/>
+      <c r="G55" s="36"/>
+      <c r="H55" s="36"/>
+      <c r="I55" s="36"/>
+      <c r="J55" s="36"/>
+      <c r="K55" s="40"/>
+      <c r="L55" s="40"/>
+      <c r="M55" s="41"/>
+      <c r="N55" s="41"/>
+      <c r="O55" s="12"/>
+      <c r="P55" s="14"/>
+      <c r="Q55" s="42"/>
     </row>
     <row r="56" spans="2:17" ht="15.75" customHeight="1">
-      <c r="B56" s="8" t="s">
-        <v>76</v>
-      </c>
-      <c r="C56" s="21"/>
-      <c r="D56" s="21"/>
-      <c r="E56" s="21"/>
-      <c r="F56" s="21"/>
-      <c r="G56" s="21"/>
-      <c r="H56" s="21"/>
-      <c r="I56" s="21"/>
-      <c r="J56" s="21"/>
-      <c r="K56" s="21"/>
-      <c r="L56" s="21"/>
-      <c r="M56" s="21"/>
-      <c r="N56" s="21"/>
-      <c r="O56" s="21"/>
-      <c r="P56" s="23"/>
-      <c r="Q56" s="23"/>
+      <c r="B56" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="C56" s="12"/>
+      <c r="D56" s="12"/>
+      <c r="E56" s="12"/>
+      <c r="F56" s="12"/>
+      <c r="G56" s="36"/>
+      <c r="H56" s="36"/>
+      <c r="I56" s="36"/>
+      <c r="J56" s="36"/>
+      <c r="K56" s="40"/>
+      <c r="L56" s="40"/>
+      <c r="M56" s="41"/>
+      <c r="N56" s="41"/>
+      <c r="O56" s="12"/>
+      <c r="P56" s="43" t="s">
+        <v>68</v>
+      </c>
+      <c r="Q56" s="42"/>
     </row>
     <row r="57" spans="2:17" ht="15.75" customHeight="1">
-      <c r="B57" s="14" t="s">
-        <v>77</v>
-      </c>
-      <c r="C57" s="12"/>
-      <c r="D57" s="12"/>
-      <c r="E57" s="12"/>
-      <c r="F57" s="12"/>
-      <c r="G57" s="12"/>
-      <c r="H57" s="12"/>
-      <c r="I57" s="12"/>
-      <c r="J57" s="12"/>
-      <c r="K57" s="12"/>
-      <c r="L57" s="20"/>
-      <c r="M57" s="20"/>
-      <c r="N57" s="20"/>
-      <c r="O57" s="46"/>
-      <c r="P57" s="14" t="s">
-        <v>78</v>
-      </c>
-      <c r="Q57" s="42"/>
+      <c r="B57" s="37" t="s">
+        <v>69</v>
+      </c>
+      <c r="C57" s="44"/>
+      <c r="D57" s="44"/>
+      <c r="E57" s="44"/>
+      <c r="F57" s="44"/>
+      <c r="G57" s="44"/>
+      <c r="H57" s="44"/>
+      <c r="I57" s="44"/>
+      <c r="J57" s="44"/>
+      <c r="K57" s="44"/>
+      <c r="L57" s="44"/>
+      <c r="M57" s="44"/>
+      <c r="N57" s="44"/>
+      <c r="O57" s="44"/>
+      <c r="P57" s="45"/>
+      <c r="Q57" s="45"/>
     </row>
     <row r="58" spans="2:17" ht="15.75" customHeight="1">
       <c r="B58" s="14" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="C58" s="12"/>
       <c r="D58" s="12"/>
       <c r="E58" s="12"/>
       <c r="F58" s="12"/>
-      <c r="G58" s="12"/>
-      <c r="H58" s="12"/>
-      <c r="I58" s="12"/>
-      <c r="J58" s="12"/>
-      <c r="K58" s="20"/>
-      <c r="L58" s="20"/>
-      <c r="M58" s="46"/>
-      <c r="N58" s="46"/>
-      <c r="O58" s="46"/>
+      <c r="G58" s="36"/>
+      <c r="H58" s="36"/>
+      <c r="I58" s="36"/>
+      <c r="J58" s="36"/>
+      <c r="K58" s="40"/>
+      <c r="L58" s="40"/>
+      <c r="M58" s="41"/>
+      <c r="N58" s="41"/>
+      <c r="O58" s="12"/>
       <c r="P58" s="14" t="s">
+        <v>71</v>
+      </c>
+      <c r="Q58" s="42"/>
+    </row>
+    <row r="59" spans="2:17" ht="15.75" customHeight="1">
+      <c r="B59" s="27" t="s">
+        <v>72</v>
+      </c>
+      <c r="C59" s="12"/>
+      <c r="D59" s="12"/>
+      <c r="E59" s="12"/>
+      <c r="F59" s="12"/>
+      <c r="G59" s="36"/>
+      <c r="H59" s="36"/>
+      <c r="I59" s="36"/>
+      <c r="J59" s="36"/>
+      <c r="K59" s="40"/>
+      <c r="L59" s="40"/>
+      <c r="M59" s="41"/>
+      <c r="N59" s="41"/>
+      <c r="O59" s="12"/>
+      <c r="P59" s="14"/>
+      <c r="Q59" s="42"/>
+    </row>
+    <row r="60" spans="2:17" ht="15.75" customHeight="1">
+      <c r="B60" s="27" t="s">
+        <v>73</v>
+      </c>
+      <c r="C60" s="12"/>
+      <c r="D60" s="12"/>
+      <c r="E60" s="12"/>
+      <c r="F60" s="12"/>
+      <c r="G60" s="36"/>
+      <c r="H60" s="36"/>
+      <c r="I60" s="36"/>
+      <c r="J60" s="36"/>
+      <c r="K60" s="40"/>
+      <c r="L60" s="40"/>
+      <c r="M60" s="41"/>
+      <c r="N60" s="41"/>
+      <c r="O60" s="12"/>
+      <c r="P60" s="14"/>
+      <c r="Q60" s="42"/>
+    </row>
+    <row r="61" spans="2:17" ht="15.75" customHeight="1">
+      <c r="B61" s="27" t="s">
+        <v>74</v>
+      </c>
+      <c r="C61" s="12"/>
+      <c r="D61" s="12"/>
+      <c r="E61" s="12"/>
+      <c r="F61" s="12"/>
+      <c r="G61" s="36"/>
+      <c r="H61" s="36"/>
+      <c r="I61" s="36"/>
+      <c r="J61" s="36"/>
+      <c r="K61" s="40"/>
+      <c r="L61" s="40"/>
+      <c r="M61" s="41"/>
+      <c r="N61" s="41"/>
+      <c r="O61" s="12"/>
+      <c r="P61" s="14"/>
+      <c r="Q61" s="42"/>
+    </row>
+    <row r="62" spans="2:17" ht="15.75" customHeight="1">
+      <c r="B62" s="56" t="s">
+        <v>75</v>
+      </c>
+      <c r="C62" s="57"/>
+      <c r="D62" s="57"/>
+      <c r="E62" s="57"/>
+      <c r="F62" s="57"/>
+      <c r="G62" s="57"/>
+      <c r="H62" s="57"/>
+      <c r="I62" s="57"/>
+      <c r="J62" s="57"/>
+      <c r="K62" s="57"/>
+      <c r="L62" s="57"/>
+      <c r="M62" s="57"/>
+      <c r="N62" s="57"/>
+      <c r="O62" s="57"/>
+      <c r="P62" s="57"/>
+      <c r="Q62" s="58"/>
+    </row>
+    <row r="63" spans="2:17" ht="15.75" customHeight="1">
+      <c r="B63" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="C63" s="21"/>
+      <c r="D63" s="21"/>
+      <c r="E63" s="21"/>
+      <c r="F63" s="21"/>
+      <c r="G63" s="21"/>
+      <c r="H63" s="21"/>
+      <c r="I63" s="21"/>
+      <c r="J63" s="21"/>
+      <c r="K63" s="21"/>
+      <c r="L63" s="21"/>
+      <c r="M63" s="21"/>
+      <c r="N63" s="21"/>
+      <c r="O63" s="21"/>
+      <c r="P63" s="23"/>
+      <c r="Q63" s="23"/>
+    </row>
+    <row r="64" spans="2:17" ht="15.75" customHeight="1">
+      <c r="B64" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="C64" s="12"/>
+      <c r="D64" s="12"/>
+      <c r="E64" s="12"/>
+      <c r="F64" s="12"/>
+      <c r="G64" s="12"/>
+      <c r="H64" s="12"/>
+      <c r="I64" s="12"/>
+      <c r="J64" s="12"/>
+      <c r="K64" s="12"/>
+      <c r="L64" s="20"/>
+      <c r="M64" s="20"/>
+      <c r="N64" s="20"/>
+      <c r="O64" s="46"/>
+      <c r="P64" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="Q64" s="42"/>
+    </row>
+    <row r="65" spans="2:17" ht="15.75" customHeight="1">
+      <c r="B65" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="C65" s="12"/>
+      <c r="D65" s="12"/>
+      <c r="E65" s="12"/>
+      <c r="F65" s="12"/>
+      <c r="G65" s="12"/>
+      <c r="H65" s="12"/>
+      <c r="I65" s="12"/>
+      <c r="J65" s="12"/>
+      <c r="K65" s="20"/>
+      <c r="L65" s="20"/>
+      <c r="M65" s="46"/>
+      <c r="N65" s="46"/>
+      <c r="O65" s="46"/>
+      <c r="P65" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="Q58" s="42"/>
-    </row>
-    <row r="59" spans="2:17" ht="15.75" customHeight="1">
-      <c r="B59" s="58" t="s">
+      <c r="Q65" s="42"/>
+    </row>
+    <row r="66" spans="2:17" ht="15.75" customHeight="1">
+      <c r="B66" s="56" t="s">
         <v>80</v>
       </c>
-      <c r="C59" s="59"/>
-      <c r="D59" s="59"/>
-      <c r="E59" s="59"/>
-      <c r="F59" s="59"/>
-      <c r="G59" s="59"/>
-      <c r="H59" s="59"/>
-      <c r="I59" s="59"/>
-      <c r="J59" s="59"/>
-      <c r="K59" s="59"/>
-      <c r="L59" s="59"/>
-      <c r="M59" s="59"/>
-      <c r="N59" s="59"/>
-      <c r="O59" s="59"/>
-      <c r="P59" s="59"/>
-      <c r="Q59" s="60"/>
-    </row>
-    <row r="60" spans="2:17" ht="15.75" customHeight="1">
-      <c r="B60" s="47"/>
-      <c r="C60" s="48"/>
-      <c r="D60" s="48"/>
-      <c r="E60" s="48"/>
-      <c r="F60" s="48"/>
-      <c r="G60" s="48"/>
-      <c r="H60" s="48"/>
-      <c r="I60" s="48"/>
-      <c r="J60" s="48"/>
-      <c r="K60" s="48"/>
-      <c r="L60" s="48"/>
-      <c r="M60" s="48"/>
-      <c r="N60" s="48"/>
-      <c r="O60" s="48"/>
-      <c r="P60" s="48"/>
-      <c r="Q60" s="48"/>
-    </row>
-    <row r="61" spans="2:17" ht="15.75" customHeight="1">
-      <c r="B61" s="49" t="s">
+      <c r="C66" s="57"/>
+      <c r="D66" s="57"/>
+      <c r="E66" s="57"/>
+      <c r="F66" s="57"/>
+      <c r="G66" s="57"/>
+      <c r="H66" s="57"/>
+      <c r="I66" s="57"/>
+      <c r="J66" s="57"/>
+      <c r="K66" s="57"/>
+      <c r="L66" s="57"/>
+      <c r="M66" s="57"/>
+      <c r="N66" s="57"/>
+      <c r="O66" s="57"/>
+      <c r="P66" s="57"/>
+      <c r="Q66" s="58"/>
+    </row>
+    <row r="67" spans="2:17" ht="15.75" customHeight="1">
+      <c r="B67" s="47"/>
+      <c r="C67" s="48"/>
+      <c r="D67" s="48"/>
+      <c r="E67" s="48"/>
+      <c r="F67" s="48"/>
+      <c r="G67" s="48"/>
+      <c r="H67" s="48"/>
+      <c r="I67" s="48"/>
+      <c r="J67" s="48"/>
+      <c r="K67" s="48"/>
+      <c r="L67" s="48"/>
+      <c r="M67" s="48"/>
+      <c r="N67" s="48"/>
+      <c r="O67" s="48"/>
+      <c r="P67" s="48"/>
+      <c r="Q67" s="48"/>
+    </row>
+    <row r="68" spans="2:17" ht="15.75" customHeight="1">
+      <c r="B68" s="49" t="s">
         <v>81</v>
       </c>
-      <c r="C61" s="48"/>
-      <c r="D61" s="48"/>
-      <c r="E61" s="48"/>
-      <c r="F61" s="48"/>
-      <c r="G61" s="48"/>
-      <c r="H61" s="48"/>
-      <c r="I61" s="48"/>
-      <c r="J61" s="48"/>
-      <c r="K61" s="48"/>
-      <c r="L61" s="48"/>
-      <c r="M61" s="48"/>
-      <c r="N61" s="48"/>
-      <c r="O61" s="48"/>
-      <c r="P61" s="48"/>
-      <c r="Q61" s="48"/>
-    </row>
-    <row r="62" spans="2:17" ht="15.75" customHeight="1"/>
-    <row r="63" spans="2:17" ht="15.75" customHeight="1">
-      <c r="B63" s="50" t="s">
+      <c r="C68" s="48"/>
+      <c r="D68" s="48"/>
+      <c r="E68" s="48"/>
+      <c r="F68" s="48"/>
+      <c r="G68" s="48"/>
+      <c r="H68" s="48"/>
+      <c r="I68" s="48"/>
+      <c r="J68" s="48"/>
+      <c r="K68" s="48"/>
+      <c r="L68" s="48"/>
+      <c r="M68" s="48"/>
+      <c r="N68" s="48"/>
+      <c r="O68" s="48"/>
+      <c r="P68" s="48"/>
+      <c r="Q68" s="48"/>
+    </row>
+    <row r="69" spans="2:17" ht="15.75" customHeight="1"/>
+    <row r="70" spans="2:17" ht="15.75" customHeight="1">
+      <c r="B70" s="50" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="64" spans="2:17" ht="15.75" customHeight="1">
-      <c r="B64" s="51" t="s">
+    <row r="71" spans="2:17" ht="15.75" customHeight="1">
+      <c r="B71" s="51" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="65" ht="15.75" customHeight="1"/>
-    <row r="66" ht="15.75" customHeight="1"/>
-    <row r="67" ht="15.75" customHeight="1"/>
-    <row r="68" ht="15.75" customHeight="1"/>
-    <row r="69" ht="15.75" customHeight="1"/>
-    <row r="70" ht="15.75" customHeight="1"/>
-    <row r="71" ht="15.75" customHeight="1"/>
-    <row r="72" ht="15.75" customHeight="1"/>
-    <row r="73" ht="15.75" customHeight="1"/>
-    <row r="74" ht="15.75" customHeight="1"/>
-    <row r="75" ht="15.75" customHeight="1"/>
-    <row r="76" ht="15.75" customHeight="1"/>
-    <row r="77" ht="15.75" customHeight="1"/>
-    <row r="78" ht="15.75" customHeight="1"/>
-    <row r="79" ht="15.75" customHeight="1"/>
-    <row r="80" ht="15.75" customHeight="1"/>
+    <row r="72" spans="2:17" ht="15.75" customHeight="1"/>
+    <row r="73" spans="2:17" ht="15.75" customHeight="1"/>
+    <row r="74" spans="2:17" ht="15.75" customHeight="1"/>
+    <row r="75" spans="2:17" ht="15.75" customHeight="1"/>
+    <row r="76" spans="2:17" ht="15.75" customHeight="1"/>
+    <row r="77" spans="2:17" ht="15.75" customHeight="1"/>
+    <row r="78" spans="2:17" ht="15.75" customHeight="1"/>
+    <row r="79" spans="2:17" ht="15.75" customHeight="1"/>
+    <row r="80" spans="2:17" ht="15.75" customHeight="1"/>
     <row r="81" ht="15.75" customHeight="1"/>
     <row r="82" ht="15.75" customHeight="1"/>
     <row r="83" ht="15.75" customHeight="1"/>
@@ -3340,24 +3549,31 @@
     <row r="1024" ht="15.75" customHeight="1"/>
     <row r="1025" ht="15.75" customHeight="1"/>
     <row r="1026" ht="15.75" customHeight="1"/>
+    <row r="1027" ht="15.75" customHeight="1"/>
+    <row r="1028" ht="15.75" customHeight="1"/>
+    <row r="1029" ht="15.75" customHeight="1"/>
+    <row r="1030" ht="15.75" customHeight="1"/>
+    <row r="1031" ht="15.75" customHeight="1"/>
+    <row r="1032" ht="15.75" customHeight="1"/>
+    <row r="1033" ht="15.75" customHeight="1"/>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="B1:Q1"/>
+    <mergeCell ref="C2:Q2"/>
+    <mergeCell ref="C3:Q3"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="E4:Q4"/>
     <mergeCell ref="C5:Q5"/>
     <mergeCell ref="I6:O6"/>
-    <mergeCell ref="B55:Q55"/>
-    <mergeCell ref="B59:Q59"/>
+    <mergeCell ref="B62:Q62"/>
+    <mergeCell ref="B66:Q66"/>
     <mergeCell ref="C6:H6"/>
     <mergeCell ref="C7:H7"/>
     <mergeCell ref="I7:O7"/>
     <mergeCell ref="C8:Q8"/>
     <mergeCell ref="C9:Q9"/>
     <mergeCell ref="B21:Q21"/>
-    <mergeCell ref="B39:Q39"/>
-    <mergeCell ref="B1:Q1"/>
-    <mergeCell ref="C2:Q2"/>
-    <mergeCell ref="C3:Q3"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="E4:Q4"/>
+    <mergeCell ref="B46:Q46"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>

</xml_diff>